<commit_message>
Added Tema 5 Sol Stat
</commit_message>
<xml_diff>
--- a/Teaching/2017-2018/PS web page/results/Tabel_Prob_Stat.xlsx
+++ b/Teaching/2017-2018/PS web page/results/Tabel_Prob_Stat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amari\OneDrive\GitHub\AlexAmarioarei.github.io\Teaching\2017-2018\PS web page\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="A1A55E76BDCFBE315C768EB27717026D88223544" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{B65331DB-7360-46B2-9347-D33CF2C4B297}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8FF3444C7F665870D3AD9D990F8B37298E07E54C" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13808" windowHeight="10605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13815" windowHeight="10605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabel_Prob_Stat" sheetId="1" r:id="rId1"/>
@@ -916,71 +916,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>495225</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>104745</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>619425</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>157125</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="4" name="Ink 3">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65C1DE63-A790-4743-A83C-627936DD60DB}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="4295700" y="1009620"/>
-            <a:ext cx="124200" cy="52380"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="4" name="Ink 3">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65C1DE63-A790-4743-A83C-627936DD60DB}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="4291020" y="1004988"/>
-              <a:ext cx="133560" cy="61288"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
       <xdr:colOff>576225</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>95175</xdr:rowOff>
@@ -993,7 +928,7 @@
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="5" name="Ink 4">
               <a:extLst>
@@ -1056,8 +991,8 @@
       <xdr:row>30</xdr:row>
       <xdr:rowOff>142905</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="9" name="Ink 8">
@@ -1076,7 +1011,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="9" name="Ink 8">
@@ -1108,384 +1043,10 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>542767</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>104745</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>552487</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>138225</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="10" name="Ink 9">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF3AE8B3-A67C-457F-A6BA-516BB12C4E9E}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="4986180" y="1009620"/>
-            <a:ext cx="9720" cy="33480"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="10" name="Ink 9">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF3AE8B3-A67C-457F-A6BA-516BB12C4E9E}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="4977180" y="1000716"/>
-              <a:ext cx="27360" cy="50932"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>595147</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>138060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>614407</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>142920</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="11" name="Ink 10">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15017D7D-DCB6-484C-B5E2-7BAD67B2EF2E}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="3095460" y="138060"/>
-            <a:ext cx="19260" cy="4860"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="11" name="Ink 10">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15017D7D-DCB6-484C-B5E2-7BAD67B2EF2E}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="3086543" y="129960"/>
-              <a:ext cx="36737" cy="20736"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>552307</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>95220</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>571567</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>104940</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="12" name="Ink 11">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65F1DA92-9FF3-4FD5-B8DC-27FE9E96BE91}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="3052620" y="95220"/>
-            <a:ext cx="19260" cy="9720"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="12" name="Ink 11">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65F1DA92-9FF3-4FD5-B8DC-27FE9E96BE91}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="3043703" y="86220"/>
-              <a:ext cx="36737" cy="27360"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>609547</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>614407</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>124020</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="15" name="Ink 14">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89156E36-2599-4010-B2E8-A92599086443}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="3109860" y="114300"/>
-            <a:ext cx="4860" cy="9720"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="15" name="Ink 14">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89156E36-2599-4010-B2E8-A92599086443}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="3105360" y="109800"/>
-              <a:ext cx="13680" cy="18540"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>585787</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>85680</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>590647</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>95400</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="16" name="Ink 15">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7AA9F1A-4D19-47D8-99AC-4BB1C3DD637A}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="3086100" y="85680"/>
-            <a:ext cx="4860" cy="9720"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="16" name="Ink 15">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7AA9F1A-4D19-47D8-99AC-4BB1C3DD637A}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="3081600" y="81180"/>
-              <a:ext cx="13680" cy="18540"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2018-02-04T20:11:06.748"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.02646" units="cm"/>
-      <inkml:brushProperty name="height" value="0.02646" units="cm"/>
-      <inkml:brushProperty name="fitToCurve" value="1"/>
-    </inkml:brush>
-    <inkml:context xml:id="ctx1">
-      <inkml:inkSource xml:id="inkSrc1">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts1" timeString="2018-02-04T20:11:09.383"/>
-    </inkml:context>
-    <inkml:brush xml:id="br1">
-      <inkml:brushProperty name="width" value="0.02646" units="cm"/>
-      <inkml:brushProperty name="height" value="0.02646" units="cm"/>
-      <inkml:brushProperty name="ignorePressure" value="1"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">73 145 1408,'-13'-14'512,"1"14"-256,12 0-384,0 0 64,-12 0-480,12 0-192</inkml:trace>
-  <inkml:trace contextRef="#ctx1" brushRef="#br1">305 118,'0'-1,"0"1,0-1,0 0,0 1,0-1,0 0,1 0,-1 1,0-1,0 0,0 1,1-1,-1 0,0 1,1-1,6-1,-7 2,3 0</inkml:trace>
-  <inkml:trace contextRef="#ctx1" brushRef="#br1" timeOffset="1">98 118,'-15'-1,"26"4,-5 3,-6-5,0-1,0 1,0-1,1 0,-1 1,0-1,0 0,1 0,-1 1,0-1,1 0,-1 0,1 1,-1-1,0 0,1 0,-1 0,1 0,-1 0,0 1,1-1,-1 0,1 0,-1 0,1 0,-1 0,0 0,1-1,-1 1,13 0</inkml:trace>
-  <inkml:trace contextRef="#ctx1" brushRef="#br1" timeOffset="2">12 13,'-12'-13,"12"13</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -1511,7 +1072,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -1535,141 +1096,6 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">13733 2911 1152,'0'-40'416,"0"27"-192,0 0-256,0 0 64,0 13-32,0-14 64,0 14-96,0 0-64</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink4.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2018-02-05T16:41:10.191"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.05" units="cm"/>
-      <inkml:brushProperty name="height" value="0.05" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">13878 2845 7296,'-13'-27'2720,"13"14"-1472,0 13-1536,0 0 448,-14 0-224,14 13-544,0 14-160,0-14-2080,0 27-928</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink5.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2018-02-05T17:46:25.258"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.05" units="cm"/>
-      <inkml:brushProperty name="height" value="0.05" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">8653 398 4736,'0'-14'1760,"-13"14"-960,-14 0-928,27 0-320,-14 0-288</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink6.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2018-02-05T17:46:26.331"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.05" units="cm"/>
-      <inkml:brushProperty name="height" value="0.05" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">8480 292 6912,'14'-27'2624,"-14"27"-1408,0 0-1408,13 13-1024,0-13-416,1 14-960,-14-14-288</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink7.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2018-02-05T17:46:27.677"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.05" units="cm"/>
-      <inkml:brushProperty name="height" value="0.05" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">8666 318 7424,'0'0'2816,"0"26"-1536,-27-26-2912,27 27-128,0-27-992,0 0-320</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink8.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2018-02-05T17:46:28.118"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.05" units="cm"/>
-      <inkml:brushProperty name="height" value="0.05" units="cm"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">8599 265 7424,'0'-27'2816,"0"27"-1536,-26 0-1568,52 0 384,-26 0-1184,0 27-480,0-27-1248,0 26-480</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1970,11 +1396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:K106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G100" sqref="G100"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2017,7 +1442,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2034,10 +1459,10 @@
         <v>61</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -2050,10 +1475,10 @@
       </c>
       <c r="K2">
         <f>MIN(10, 1+0.5*J2+0.2*I2+0.06*(C2/9+D2/7+E2/7+F2/7+G2/6))</f>
-        <v>2.578095238095238</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.6323809523809523</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2070,10 +1495,10 @@
         <v>53</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -2086,10 +1511,10 @@
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K66" si="0">MIN(10, 1+0.5*J3+0.2*I3+0.06*(C3/9+D3/7+E3/7+F3/7+G3/6))</f>
-        <v>2.3219047619047619</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.2976190476190479</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -2106,10 +1531,10 @@
         <v>62</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -2122,10 +1547,10 @@
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>2.4628571428571426</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.407142857142857</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2161,7 +1586,7 @@
         <v>1.4466666666666668</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -2175,13 +1600,13 @@
         <v>61</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -2194,10 +1619,10 @@
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>1.8561904761904762</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>2.7604761904761905</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2214,10 +1639,10 @@
         <v>44</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -2230,10 +1655,10 @@
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>2.1799999999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>2.9828571428571431</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -2253,7 +1678,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -2266,10 +1691,10 @@
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>1.92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>2.4499999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -2305,7 +1730,7 @@
         <v>1.6819047619047618</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2325,7 +1750,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -2338,10 +1763,10 @@
       </c>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>2.3952380952380952</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>2.9552380952380952</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -2377,7 +1802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -2394,10 +1819,10 @@
         <v>46</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -2410,10 +1835,10 @@
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>2.1342857142857143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>2.8085714285714287</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2430,10 +1855,10 @@
         <v>55</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -2446,10 +1871,10 @@
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>2.5466666666666669</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.5595238095238093</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -2466,10 +1891,10 @@
         <v>58</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -2482,10 +1907,10 @@
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>2.5828571428571427</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.621428571428571</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -2502,10 +1927,10 @@
         <v>57</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -2518,10 +1943,10 @@
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>2.4466666666666663</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.1409523809523812</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -2557,7 +1982,7 @@
         <v>1.5085714285714285</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -2577,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -2590,10 +2015,10 @@
       </c>
       <c r="K17">
         <f t="shared" si="0"/>
-        <v>1.7000000000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -2610,10 +2035,10 @@
         <v>58</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -2626,10 +2051,10 @@
       </c>
       <c r="K18">
         <f t="shared" si="0"/>
-        <v>2.5742857142857143</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.6014285714285714</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -2646,10 +2071,10 @@
         <v>30</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -2662,10 +2087,10 @@
       </c>
       <c r="K19">
         <f t="shared" si="0"/>
-        <v>2.059047619047619</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>2.7519047619047621</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -2701,7 +2126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -2718,10 +2143,10 @@
         <v>61</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -2734,10 +2159,10 @@
       </c>
       <c r="K21">
         <f t="shared" si="0"/>
-        <v>2.6152380952380954</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.686666666666667</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -2773,7 +2198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -2790,10 +2215,10 @@
         <v>54</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -2806,10 +2231,10 @@
       </c>
       <c r="K23">
         <f t="shared" si="0"/>
-        <v>2.5133333333333332</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.4647619047619043</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -2845,7 +2270,7 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -2881,7 +2306,7 @@
         <v>1.8685714285714283</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -2901,7 +2326,7 @@
         <v>0</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -2914,10 +2339,10 @@
       </c>
       <c r="K26">
         <f t="shared" si="0"/>
-        <v>2.1019047619047617</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>2.5419047619047621</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -2934,10 +2359,10 @@
         <v>46</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -2950,10 +2375,10 @@
       </c>
       <c r="K27">
         <f t="shared" si="0"/>
-        <v>1.8542857142857141</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>2.8199999999999994</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -2970,10 +2395,10 @@
         <v>55</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -2986,10 +2411,10 @@
       </c>
       <c r="K28">
         <f t="shared" si="0"/>
-        <v>2.5742857142857138</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.4699999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -3006,7 +2431,7 @@
         <v>57</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -3022,10 +2447,10 @@
       </c>
       <c r="K29">
         <f t="shared" si="0"/>
-        <v>2.5876190476190475</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.0847619047619048</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -3061,7 +2486,7 @@
         <v>1.5104761904761905</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -3081,7 +2506,7 @@
         <v>0</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -3094,10 +2519,10 @@
       </c>
       <c r="K31">
         <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.0199999999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -3133,7 +2558,7 @@
         <v>1.5161904761904763</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -3153,7 +2578,7 @@
         <v>0</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -3166,10 +2591,10 @@
       </c>
       <c r="K33">
         <f t="shared" si="0"/>
-        <v>2.3047619047619046</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>2.8247619047619046</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -3186,10 +2611,10 @@
         <v>44</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="H34">
         <v>0</v>
@@ -3202,10 +2627,10 @@
       </c>
       <c r="K34">
         <f t="shared" si="0"/>
-        <v>2.2285714285714286</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.1671428571428573</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -3222,10 +2647,10 @@
         <v>46</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -3238,10 +2663,10 @@
       </c>
       <c r="K35">
         <f t="shared" si="0"/>
-        <v>2.3199999999999998</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.2857142857142856</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -3277,7 +2702,7 @@
         <v>1.7714285714285714</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -3313,7 +2738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -3330,10 +2755,10 @@
         <v>57</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -3346,10 +2771,10 @@
       </c>
       <c r="K38">
         <f t="shared" si="0"/>
-        <v>2.157142857142857</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.0457142857142858</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -3369,7 +2794,7 @@
         <v>0</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -3382,10 +2807,10 @@
       </c>
       <c r="K39">
         <f t="shared" si="0"/>
-        <v>1.5257142857142858</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>1.9157142857142857</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -3402,10 +2827,10 @@
         <v>55</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -3418,10 +2843,10 @@
       </c>
       <c r="K40">
         <f t="shared" si="0"/>
-        <v>2.5038095238095237</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.582380952380952</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>50</v>
       </c>
@@ -3441,7 +2866,7 @@
         <v>0</v>
       </c>
       <c r="G41">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -3454,10 +2879,10 @@
       </c>
       <c r="K41">
         <f t="shared" si="0"/>
-        <v>1.6590476190476191</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>2.1890476190476189</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>51</v>
       </c>
@@ -3474,10 +2899,10 @@
         <v>43</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -3490,10 +2915,10 @@
       </c>
       <c r="K42">
         <f t="shared" si="0"/>
-        <v>1.9523809523809523</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>2.6166666666666663</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -3529,7 +2954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -3549,7 +2974,7 @@
         <v>0</v>
       </c>
       <c r="G44">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="H44">
         <v>0</v>
@@ -3562,10 +2987,10 @@
       </c>
       <c r="K44">
         <f t="shared" si="0"/>
-        <v>1.6523809523809523</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>2.0123809523809522</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -3582,7 +3007,7 @@
         <v>57</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -3598,10 +3023,10 @@
       </c>
       <c r="K45">
         <f t="shared" si="0"/>
-        <v>2.4257142857142857</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>2.862857142857143</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -3621,7 +3046,7 @@
         <v>0</v>
       </c>
       <c r="G46">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -3634,10 +3059,10 @@
       </c>
       <c r="K46">
         <f t="shared" si="0"/>
-        <v>2.5838095238095238</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.113809523809524</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>56</v>
       </c>
@@ -3654,10 +3079,10 @@
         <v>59</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -3670,10 +3095,10 @@
       </c>
       <c r="K47">
         <f t="shared" si="0"/>
-        <v>2.5666666666666669</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.6109523809523809</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>57</v>
       </c>
@@ -3690,7 +3115,7 @@
         <v>43</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -3706,10 +3131,10 @@
       </c>
       <c r="K48">
         <f t="shared" si="0"/>
-        <v>1.7752380952380953</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>2.0152380952380953</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>58</v>
       </c>
@@ -3745,7 +3170,7 @@
         <v>2.0285714285714285</v>
       </c>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>59</v>
       </c>
@@ -3762,10 +3187,10 @@
         <v>57</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -3778,10 +3203,10 @@
       </c>
       <c r="K50">
         <f t="shared" si="0"/>
-        <v>2.3199999999999998</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.4042857142857139</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>60</v>
       </c>
@@ -3817,7 +3242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>61</v>
       </c>
@@ -3834,10 +3259,10 @@
         <v>59</v>
       </c>
       <c r="F52">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -3850,10 +3275,10 @@
       </c>
       <c r="K52">
         <f t="shared" si="0"/>
-        <v>2.0523809523809522</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.1295238095238092</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>62</v>
       </c>
@@ -3870,10 +3295,10 @@
         <v>56</v>
       </c>
       <c r="F53">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="G53">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H53">
         <v>0</v>
@@ -3886,10 +3311,10 @@
       </c>
       <c r="K53">
         <f t="shared" si="0"/>
-        <v>2.5066666666666668</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.6009523809523807</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>63</v>
       </c>
@@ -3925,7 +3350,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -3942,7 +3367,7 @@
         <v>37</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -3958,10 +3383,10 @@
       </c>
       <c r="K55">
         <f t="shared" si="0"/>
-        <v>1.9561904761904763</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>2.3419047619047619</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>65</v>
       </c>
@@ -3978,10 +3403,10 @@
         <v>52</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="G56">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H56">
         <v>0</v>
@@ -3994,10 +3419,10 @@
       </c>
       <c r="K56">
         <f t="shared" si="0"/>
-        <v>2.4257142857142862</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.3571428571428572</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>66</v>
       </c>
@@ -4033,7 +3458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>67</v>
       </c>
@@ -4069,7 +3494,7 @@
         <v>1.5495238095238095</v>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>68</v>
       </c>
@@ -4105,7 +3530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>69</v>
       </c>
@@ -4122,10 +3547,10 @@
         <v>58</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="G60">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -4138,10 +3563,10 @@
       </c>
       <c r="K60">
         <f t="shared" si="0"/>
-        <v>2.4609523809523806</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.5209523809523806</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -4158,10 +3583,10 @@
         <v>56</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="G61">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -4174,10 +3599,10 @@
       </c>
       <c r="K61">
         <f t="shared" si="0"/>
-        <v>2.4533333333333331</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.47047619047619</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>71</v>
       </c>
@@ -4213,7 +3638,7 @@
         <v>1.7314285714285713</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>72</v>
       </c>
@@ -4230,10 +3655,10 @@
         <v>58</v>
       </c>
       <c r="F63">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="G63">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H63">
         <v>0</v>
@@ -4246,10 +3671,10 @@
       </c>
       <c r="K63">
         <f t="shared" si="0"/>
-        <v>2.5857142857142859</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.6714285714285713</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>73</v>
       </c>
@@ -4266,10 +3691,10 @@
         <v>55</v>
       </c>
       <c r="F64">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="G64">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -4282,10 +3707,10 @@
       </c>
       <c r="K64">
         <f t="shared" si="0"/>
-        <v>2.5095238095238095</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.5866666666666669</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>74</v>
       </c>
@@ -4302,10 +3727,10 @@
         <v>58</v>
       </c>
       <c r="F65">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="G65">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H65">
         <v>0</v>
@@ -4318,10 +3743,10 @@
       </c>
       <c r="K65">
         <f t="shared" si="0"/>
-        <v>2.5723809523809527</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.6495238095238092</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>75</v>
       </c>
@@ -4341,7 +3766,7 @@
         <v>0</v>
       </c>
       <c r="G66">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -4354,10 +3779,10 @@
       </c>
       <c r="K66">
         <f t="shared" si="0"/>
-        <v>2.3857142857142857</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>2.9057142857142857</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>76</v>
       </c>
@@ -4374,10 +3799,10 @@
         <v>57</v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="G67">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -4390,10 +3815,10 @@
       </c>
       <c r="K67">
         <f t="shared" ref="K67:K106" si="1">MIN(10, 1+0.5*J67+0.2*I67+0.06*(C67/9+D67/7+E67/7+F67/7+G67/6))</f>
-        <v>2.5438095238095237</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.6123809523809522</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>77</v>
       </c>
@@ -4410,10 +3835,10 @@
         <v>57</v>
       </c>
       <c r="F68">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="G68">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -4426,10 +3851,10 @@
       </c>
       <c r="K68">
         <f t="shared" si="1"/>
-        <v>2.5571428571428569</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.6257142857142854</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>78</v>
       </c>
@@ -4465,7 +3890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>79</v>
       </c>
@@ -4501,7 +3926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>80</v>
       </c>
@@ -4518,10 +3943,10 @@
         <v>53</v>
       </c>
       <c r="F71">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="G71">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -4534,10 +3959,10 @@
       </c>
       <c r="K71">
         <f t="shared" si="1"/>
-        <v>2.5076190476190474</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>3.5933333333333333</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>81</v>
       </c>
@@ -4554,7 +3979,7 @@
         <v>39</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="G72">
         <v>0</v>
@@ -4570,10 +3995,10 @@
       </c>
       <c r="K72">
         <f t="shared" si="1"/>
-        <v>1.6342857142857143</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>2.1314285714285717</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>82</v>
       </c>
@@ -4590,10 +4015,10 @@
         <v>57</v>
       </c>
       <c r="F73">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="G73">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H73">
         <v>0</v>
@@ -4606,7 +4031,7 @@
       </c>
       <c r="K73">
         <f t="shared" si="1"/>
-        <v>2.4257142857142857</v>
+        <v>3.4942857142857142</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.45">
@@ -4665,7 +4090,7 @@
         <v>0</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H75">
         <v>0</v>
@@ -4678,7 +4103,7 @@
       </c>
       <c r="K75">
         <f t="shared" si="1"/>
-        <v>1.6666666666666665</v>
+        <v>2.1966666666666663</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.45">
@@ -4698,10 +4123,10 @@
         <v>58</v>
       </c>
       <c r="F76">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="G76">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="H76">
         <v>0</v>
@@ -4714,7 +4139,7 @@
       </c>
       <c r="K76">
         <f t="shared" si="1"/>
-        <v>2.6552380952380954</v>
+        <v>3.808095238095238</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.45">
@@ -4734,10 +4159,10 @@
         <v>0</v>
       </c>
       <c r="F77">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="G77">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="H77">
         <v>0</v>
@@ -4750,7 +4175,7 @@
       </c>
       <c r="K77">
         <f t="shared" si="1"/>
-        <v>1.3257142857142856</v>
+        <v>2.1642857142857146</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.45">
@@ -4770,10 +4195,10 @@
         <v>48</v>
       </c>
       <c r="F78">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="G78">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H78">
         <v>0</v>
@@ -4786,7 +4211,7 @@
       </c>
       <c r="K78">
         <f t="shared" si="1"/>
-        <v>1.7914285714285714</v>
+        <v>2.7671428571428573</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.45">
@@ -4806,10 +4231,10 @@
         <v>59</v>
       </c>
       <c r="F79">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="G79">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H79">
         <v>0</v>
@@ -4822,7 +4247,7 @@
       </c>
       <c r="K79">
         <f t="shared" si="1"/>
-        <v>2.5914285714285716</v>
+        <v>3.652857142857143</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.45">
@@ -4842,10 +4267,10 @@
         <v>38</v>
       </c>
       <c r="F80">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="G80">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H80">
         <v>0</v>
@@ -4858,7 +4283,7 @@
       </c>
       <c r="K80">
         <f t="shared" si="1"/>
-        <v>2.1828571428571428</v>
+        <v>2.9428571428571426</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.45">
@@ -4878,10 +4303,10 @@
         <v>60</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="G81">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="H81">
         <v>0</v>
@@ -4894,7 +4319,7 @@
       </c>
       <c r="K81">
         <f t="shared" si="1"/>
-        <v>2.6047619047619048</v>
+        <v>3.583333333333333</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.45">
@@ -4914,10 +4339,10 @@
         <v>0</v>
       </c>
       <c r="F82">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="G82">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H82">
         <v>0</v>
@@ -4930,7 +4355,7 @@
       </c>
       <c r="K82">
         <f t="shared" si="1"/>
-        <v>1.5742857142857143</v>
+        <v>2.524285714285714</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.45">
@@ -4986,10 +4411,10 @@
         <v>57</v>
       </c>
       <c r="F84">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="G84">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H84">
         <v>0</v>
@@ -5002,7 +4427,7 @@
       </c>
       <c r="K84">
         <f t="shared" si="1"/>
-        <v>2.411428571428571</v>
+        <v>3.4471428571428571</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.45">
@@ -5022,10 +4447,10 @@
         <v>59</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="G85">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H85">
         <v>0</v>
@@ -5038,7 +4463,7 @@
       </c>
       <c r="K85">
         <f t="shared" si="1"/>
-        <v>2.4885714285714284</v>
+        <v>3.4814285714285718</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.45">
@@ -5061,7 +4486,7 @@
         <v>0</v>
       </c>
       <c r="G86">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H86">
         <v>0</v>
@@ -5074,7 +4499,7 @@
       </c>
       <c r="K86">
         <f t="shared" si="1"/>
-        <v>1.9885714285714284</v>
+        <v>2.5185714285714287</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.45">
@@ -5130,7 +4555,7 @@
         <v>23</v>
       </c>
       <c r="F88">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G88">
         <v>0</v>
@@ -5146,7 +4571,7 @@
       </c>
       <c r="K88">
         <f t="shared" si="1"/>
-        <v>2.0647619047619048</v>
+        <v>2.2619047619047619</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.45">
@@ -5166,10 +4591,10 @@
         <v>61</v>
       </c>
       <c r="F89">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="G89">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="H89">
         <v>0</v>
@@ -5182,7 +4607,7 @@
       </c>
       <c r="K89">
         <f t="shared" si="1"/>
-        <v>2.6390476190476191</v>
+        <v>3.7104761904761907</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.45">
@@ -5202,10 +4627,10 @@
         <v>57</v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="G90">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H90">
         <v>0</v>
@@ -5218,7 +4643,7 @@
       </c>
       <c r="K90">
         <f t="shared" si="1"/>
-        <v>2.2838095238095235</v>
+        <v>3.2766666666666664</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.45">
@@ -5238,7 +4663,7 @@
         <v>49</v>
       </c>
       <c r="F91">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -5254,7 +4679,7 @@
       </c>
       <c r="K91">
         <f t="shared" si="1"/>
-        <v>2.3590476190476188</v>
+        <v>2.7790476190476188</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.45">
@@ -5274,10 +4699,10 @@
         <v>59</v>
       </c>
       <c r="F92">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="G92">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H92">
         <v>0</v>
@@ -5290,7 +4715,7 @@
       </c>
       <c r="K92">
         <f t="shared" si="1"/>
-        <v>2.6419047619047618</v>
+        <v>3.7190476190476187</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.45">
@@ -5310,10 +4735,10 @@
         <v>58</v>
       </c>
       <c r="F93">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="G93">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="H93">
         <v>0</v>
@@ -5326,7 +4751,7 @@
       </c>
       <c r="K93">
         <f t="shared" si="1"/>
-        <v>2.6466666666666665</v>
+        <v>3.7352380952380946</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.45">
@@ -5346,10 +4771,10 @@
         <v>28</v>
       </c>
       <c r="F94">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="G94">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H94">
         <v>0</v>
@@ -5362,7 +4787,7 @@
       </c>
       <c r="K94">
         <f t="shared" si="1"/>
-        <v>2.1323809523809523</v>
+        <v>2.9538095238095234</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.45">
@@ -5382,10 +4807,10 @@
         <v>49</v>
       </c>
       <c r="F95">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="G95">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H95">
         <v>0</v>
@@ -5398,7 +4823,7 @@
       </c>
       <c r="K95">
         <f t="shared" si="1"/>
-        <v>2.3076190476190477</v>
+        <v>3.2833333333333332</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.45">
@@ -5418,10 +4843,10 @@
         <v>59</v>
       </c>
       <c r="F96">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="G96">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H96">
         <v>0</v>
@@ -5434,7 +4859,7 @@
       </c>
       <c r="K96">
         <f t="shared" si="1"/>
-        <v>2.5933333333333333</v>
+        <v>3.6547619047619051</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.45">
@@ -5454,10 +4879,10 @@
         <v>59</v>
       </c>
       <c r="F97">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="G97">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H97">
         <v>0</v>
@@ -5470,7 +4895,7 @@
       </c>
       <c r="K97">
         <f t="shared" si="1"/>
-        <v>2.5019047619047621</v>
+        <v>3.494761904761905</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.45">
@@ -5490,10 +4915,10 @@
         <v>59</v>
       </c>
       <c r="F98">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="G98">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H98">
         <v>0</v>
@@ -5506,7 +4931,7 @@
       </c>
       <c r="K98">
         <f t="shared" si="1"/>
-        <v>2.5999999999999996</v>
+        <v>3.67</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.45">
@@ -5526,10 +4951,10 @@
         <v>45</v>
       </c>
       <c r="F99">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G99">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H99">
         <v>0</v>
@@ -5542,7 +4967,7 @@
       </c>
       <c r="K99">
         <f t="shared" si="1"/>
-        <v>2.3552380952380956</v>
+        <v>3.0295238095238095</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.45">
@@ -5598,10 +5023,10 @@
         <v>59</v>
       </c>
       <c r="F101">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="G101">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H101">
         <v>0</v>
@@ -5614,7 +5039,7 @@
       </c>
       <c r="K101">
         <f t="shared" si="1"/>
-        <v>2.5847619047619048</v>
+        <v>3.671904761904762</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.45">
@@ -5634,10 +5059,10 @@
         <v>58</v>
       </c>
       <c r="F102">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="G102">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H102">
         <v>0</v>
@@ -5650,7 +5075,7 @@
       </c>
       <c r="K102">
         <f t="shared" si="1"/>
-        <v>2.5914285714285716</v>
+        <v>3.6357142857142857</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.45">
@@ -5673,7 +5098,7 @@
         <v>0</v>
       </c>
       <c r="G103">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="H103">
         <v>0</v>
@@ -5686,7 +5111,7 @@
       </c>
       <c r="K103">
         <f t="shared" si="1"/>
-        <v>2.2285714285714286</v>
+        <v>2.7585714285714285</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.45">
@@ -5706,10 +5131,10 @@
         <v>60</v>
       </c>
       <c r="F104">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="G104">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="H104">
         <v>0</v>
@@ -5722,7 +5147,7 @@
       </c>
       <c r="K104">
         <f t="shared" si="1"/>
-        <v>2.54</v>
+        <v>3.2899999999999996</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.45">
@@ -5742,10 +5167,10 @@
         <v>30</v>
       </c>
       <c r="F105">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="G105">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="H105">
         <v>0</v>
@@ -5758,10 +5183,10 @@
       </c>
       <c r="K105">
         <f t="shared" si="1"/>
-        <v>1.2571428571428571</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>114</v>
       </c>
@@ -5778,10 +5203,10 @@
         <v>42</v>
       </c>
       <c r="F106">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="G106">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="H106">
         <v>0</v>
@@ -5794,17 +5219,11 @@
       </c>
       <c r="K106">
         <f t="shared" si="1"/>
-        <v>1.6514285714285715</v>
+        <v>2.3714285714285714</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K106" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="244"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K106" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update results 301 Stat
</commit_message>
<xml_diff>
--- a/Teaching/2017-2018/PS web page/results/Tabel_Prob_Stat.xlsx
+++ b/Teaching/2017-2018/PS web page/results/Tabel_Prob_Stat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amari\OneDrive\GitHub\AlexAmarioarei.github.io\Teaching\2017-2018\PS web page\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8FF3444C7F665870D3AD9D990F8B37298E07E54C" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="8FF3444C7F665870D3AD9D990F8B37298E07E54C" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{B201E90F-CCF8-423C-9691-9374B0CB9082}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13815" windowHeight="10605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Tabel_Prob_Stat" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabel_Prob_Stat!$A$1:$K$106</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabel_Prob_Stat!$A$1:$J$106</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="114">
   <si>
     <t>Nume</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>Tema_5</t>
-  </si>
-  <si>
-    <t>Tema_6</t>
   </si>
   <si>
     <t>Proiect</t>
@@ -1396,10 +1393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K106"/>
+  <dimension ref="A1:J106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="I76" sqref="I76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1407,7 +1404,7 @@
     <col min="1" max="1" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1438,13 +1435,10 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>11</v>
       </c>
       <c r="B2">
         <v>241</v>
@@ -1468,19 +1462,16 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <f>MIN(10, 1+0.5*J2+0.2*I2+0.06*(C2/9+D2/7+E2/7+F2/7+G2/6))</f>
-        <v>3.6323809523809523</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+        <f>MIN(10, 1+0.5*I2/5+0.2*H2+0.06*(C2/9+D2/7+E2/7+F2/7+G2/6))</f>
+        <v>6.7323809523809519</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>241</v>
@@ -1504,19 +1495,16 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K66" si="0">MIN(10, 1+0.5*J3+0.2*I3+0.06*(C3/9+D3/7+E3/7+F3/7+G3/6))</f>
-        <v>3.2976190476190479</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" ref="J3:J66" si="0">MIN(10, 1+0.5*I3/5+0.2*H3+0.06*(C3/9+D3/7+E3/7+F3/7+G3/6))</f>
+        <v>5.7976190476190474</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>241</v>
@@ -1540,19 +1528,16 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="0"/>
-        <v>3.407142857142857</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>5.1071428571428577</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>241</v>
@@ -1576,19 +1561,16 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
-        <v>1.4466666666666668</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>2.1466666666666665</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>241</v>
@@ -1612,19 +1594,16 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
-        <v>2.7604761904761905</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>3.9604761904761907</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>241</v>
@@ -1648,19 +1627,16 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="0"/>
-        <v>2.9828571428571431</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>4.9828571428571431</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>241</v>
@@ -1684,19 +1660,16 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="0"/>
-        <v>2.4499999999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>241</v>
@@ -1720,19 +1693,16 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="0"/>
-        <v>1.6819047619047618</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>1.7819047619047619</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>241</v>
@@ -1756,19 +1726,16 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="0"/>
-        <v>2.9552380952380952</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>3.0552380952380953</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>241</v>
@@ -1795,16 +1762,13 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>241</v>
@@ -1828,19 +1792,16 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="0"/>
-        <v>2.8085714285714287</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>4.2085714285714282</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>241</v>
@@ -1864,19 +1825,16 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="0"/>
-        <v>3.5595238095238093</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>5.6595238095238098</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>241</v>
@@ -1896,23 +1854,17 @@
       <c r="G14">
         <v>55</v>
       </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
       <c r="I14">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="0"/>
-        <v>3.621428571428571</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>6.121428571428571</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>241</v>
@@ -1939,16 +1891,13 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
         <f t="shared" si="0"/>
         <v>3.1409523809523812</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>241</v>
@@ -1972,19 +1921,16 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="0"/>
-        <v>1.5085714285714285</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>3.4085714285714284</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>241</v>
@@ -2008,19 +1954,16 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="0"/>
-        <v>2.11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>3.4099999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>241</v>
@@ -2044,19 +1987,16 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="0"/>
-        <v>3.6014285714285714</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>5.4014285714285712</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>241</v>
@@ -2080,19 +2020,16 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="0"/>
-        <v>2.7519047619047621</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>4.7519047619047621</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20">
         <v>241</v>
@@ -2119,16 +2056,13 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21">
         <v>241</v>
@@ -2152,19 +2086,16 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="0"/>
-        <v>3.686666666666667</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>5.7866666666666671</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22">
         <v>241</v>
@@ -2191,16 +2122,13 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23">
         <v>241</v>
@@ -2224,19 +2152,16 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="0"/>
-        <v>3.4647619047619043</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>5.3647619047619042</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24">
         <v>241</v>
@@ -2245,10 +2170,10 @@
         <v>63</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -2260,19 +2185,16 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="0"/>
-        <v>1.42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>3.097142857142857</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25">
         <v>241</v>
@@ -2296,19 +2218,16 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <f t="shared" si="0"/>
-        <v>1.8685714285714283</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>2.9685714285714284</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26">
         <v>241</v>
@@ -2335,16 +2254,13 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26">
         <f t="shared" si="0"/>
         <v>2.5419047619047621</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27">
         <v>242</v>
@@ -2368,19 +2284,16 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J27">
-        <v>0</v>
-      </c>
-      <c r="K27">
-        <f t="shared" si="0"/>
-        <v>2.8199999999999994</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>4.8199999999999994</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28">
         <v>242</v>
@@ -2404,19 +2317,16 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <f t="shared" si="0"/>
-        <v>3.4699999999999998</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>4.3699999999999992</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29">
         <v>242</v>
@@ -2440,19 +2350,16 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <f t="shared" si="0"/>
-        <v>3.0847619047619048</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>4.4847619047619052</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30">
         <v>242</v>
@@ -2476,19 +2383,16 @@
         <v>0</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J30">
-        <v>0</v>
-      </c>
-      <c r="K30">
-        <f t="shared" si="0"/>
-        <v>1.5104761904761905</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>2.2104761904761903</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31">
         <v>242</v>
@@ -2512,19 +2416,16 @@
         <v>0</v>
       </c>
       <c r="I31">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="J31">
-        <v>0</v>
-      </c>
-      <c r="K31">
-        <f t="shared" si="0"/>
-        <v>3.0199999999999996</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>4.92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32">
         <v>242</v>
@@ -2551,16 +2452,13 @@
         <v>0</v>
       </c>
       <c r="J32">
-        <v>0</v>
-      </c>
-      <c r="K32">
         <f t="shared" si="0"/>
         <v>1.5161904761904763</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33">
         <v>242</v>
@@ -2584,19 +2482,16 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="J33">
-        <v>0</v>
-      </c>
-      <c r="K33">
-        <f t="shared" si="0"/>
-        <v>2.8247619047619046</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>5.0247619047619043</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34">
         <v>242</v>
@@ -2620,19 +2515,16 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="J34">
-        <v>0</v>
-      </c>
-      <c r="K34">
-        <f t="shared" si="0"/>
-        <v>3.1671428571428573</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>5.2671428571428578</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35">
         <v>242</v>
@@ -2656,19 +2548,16 @@
         <v>0</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="J35">
-        <v>0</v>
-      </c>
-      <c r="K35">
-        <f t="shared" si="0"/>
-        <v>3.2857142857142856</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>4.9857142857142858</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36">
         <v>242</v>
@@ -2692,19 +2581,16 @@
         <v>0</v>
       </c>
       <c r="I36">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J36">
-        <v>0</v>
-      </c>
-      <c r="K36">
-        <f t="shared" si="0"/>
-        <v>1.7714285714285714</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>3.1714285714285713</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B37">
         <v>242</v>
@@ -2728,19 +2614,16 @@
         <v>0</v>
       </c>
       <c r="I37">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J37">
-        <v>0</v>
-      </c>
-      <c r="K37">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B38">
         <v>242</v>
@@ -2764,19 +2647,16 @@
         <v>0</v>
       </c>
       <c r="I38">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J38">
-        <v>0</v>
-      </c>
-      <c r="K38">
-        <f t="shared" si="0"/>
-        <v>3.0457142857142858</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>4.0457142857142863</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B39">
         <v>242</v>
@@ -2803,16 +2683,13 @@
         <v>0</v>
       </c>
       <c r="J39">
-        <v>0</v>
-      </c>
-      <c r="K39">
         <f t="shared" si="0"/>
         <v>1.9157142857142857</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B40">
         <v>242</v>
@@ -2836,19 +2713,16 @@
         <v>0</v>
       </c>
       <c r="I40">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J40">
-        <v>0</v>
-      </c>
-      <c r="K40">
-        <f t="shared" si="0"/>
-        <v>3.582380952380952</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>5.5823809523809516</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B41">
         <v>242</v>
@@ -2875,16 +2749,13 @@
         <v>0</v>
       </c>
       <c r="J41">
-        <v>0</v>
-      </c>
-      <c r="K41">
         <f t="shared" si="0"/>
         <v>2.1890476190476189</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B42">
         <v>242</v>
@@ -2908,19 +2779,16 @@
         <v>0</v>
       </c>
       <c r="I42">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J42">
-        <v>0</v>
-      </c>
-      <c r="K42">
-        <f t="shared" si="0"/>
-        <v>2.6166666666666663</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>4.2166666666666668</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B43">
         <v>242</v>
@@ -2947,16 +2815,13 @@
         <v>0</v>
       </c>
       <c r="J43">
-        <v>0</v>
-      </c>
-      <c r="K43">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B44">
         <v>242</v>
@@ -2983,16 +2848,13 @@
         <v>0</v>
       </c>
       <c r="J44">
-        <v>0</v>
-      </c>
-      <c r="K44">
         <f t="shared" si="0"/>
         <v>2.0123809523809522</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B45">
         <v>242</v>
@@ -3016,19 +2878,16 @@
         <v>0</v>
       </c>
       <c r="I45">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J45">
-        <v>0</v>
-      </c>
-      <c r="K45">
-        <f t="shared" si="0"/>
-        <v>2.862857142857143</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>4.6628571428571428</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B46">
         <v>242</v>
@@ -3052,19 +2911,16 @@
         <v>0</v>
       </c>
       <c r="I46">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="J46">
-        <v>0</v>
-      </c>
-      <c r="K46">
-        <f t="shared" si="0"/>
-        <v>3.113809523809524</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>5.3138095238095246</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B47">
         <v>242</v>
@@ -3088,19 +2944,16 @@
         <v>0</v>
       </c>
       <c r="I47">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J47">
-        <v>0</v>
-      </c>
-      <c r="K47">
-        <f t="shared" si="0"/>
-        <v>3.6109523809523809</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>6.6109523809523809</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B48">
         <v>242</v>
@@ -3127,16 +2980,13 @@
         <v>0</v>
       </c>
       <c r="J48">
-        <v>0</v>
-      </c>
-      <c r="K48">
         <f t="shared" si="0"/>
         <v>2.0152380952380953</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B49">
         <v>243</v>
@@ -3160,19 +3010,16 @@
         <v>0</v>
       </c>
       <c r="I49">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J49">
-        <v>0</v>
-      </c>
-      <c r="K49">
-        <f t="shared" si="0"/>
-        <v>2.0285714285714285</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>3.4285714285714284</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B50">
         <v>243</v>
@@ -3196,19 +3043,16 @@
         <v>0</v>
       </c>
       <c r="I50">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="J50">
-        <v>0</v>
-      </c>
-      <c r="K50">
-        <f t="shared" si="0"/>
-        <v>3.4042857142857139</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>6.2042857142857137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B51">
         <v>243</v>
@@ -3235,16 +3079,13 @@
         <v>0</v>
       </c>
       <c r="J51">
-        <v>0</v>
-      </c>
-      <c r="K51">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B52">
         <v>243</v>
@@ -3268,19 +3109,16 @@
         <v>0</v>
       </c>
       <c r="I52">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="J52">
-        <v>0</v>
-      </c>
-      <c r="K52">
-        <f t="shared" si="0"/>
-        <v>3.1295238095238092</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>5.2295238095238092</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B53">
         <v>243</v>
@@ -3304,19 +3142,16 @@
         <v>0</v>
       </c>
       <c r="I53">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="J53">
-        <v>0</v>
-      </c>
-      <c r="K53">
-        <f t="shared" si="0"/>
-        <v>3.6009523809523807</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>6.3009523809523813</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B54">
         <v>243</v>
@@ -3343,16 +3178,13 @@
         <v>0</v>
       </c>
       <c r="J54">
-        <v>0</v>
-      </c>
-      <c r="K54">
         <f t="shared" si="0"/>
         <v>1.48</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B55">
         <v>243</v>
@@ -3376,19 +3208,16 @@
         <v>0</v>
       </c>
       <c r="I55">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="J55">
-        <v>0</v>
-      </c>
-      <c r="K55">
-        <f t="shared" si="0"/>
-        <v>2.3419047619047619</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>4.9419047619047625</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B56">
         <v>243</v>
@@ -3412,19 +3241,16 @@
         <v>0</v>
       </c>
       <c r="I56">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="J56">
-        <v>0</v>
-      </c>
-      <c r="K56">
-        <f t="shared" si="0"/>
-        <v>3.3571428571428572</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>6.1571428571428566</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B57">
         <v>243</v>
@@ -3448,19 +3274,16 @@
         <v>0</v>
       </c>
       <c r="I57">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J57">
-        <v>0</v>
-      </c>
-      <c r="K57">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B58">
         <v>243</v>
@@ -3484,19 +3307,16 @@
         <v>0</v>
       </c>
       <c r="I58">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J58">
-        <v>0</v>
-      </c>
-      <c r="K58">
-        <f t="shared" si="0"/>
-        <v>1.5495238095238095</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>1.9495238095238094</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B59">
         <v>243</v>
@@ -3520,19 +3340,16 @@
         <v>0</v>
       </c>
       <c r="I59">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J59">
-        <v>0</v>
-      </c>
-      <c r="K59">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B60">
         <v>243</v>
@@ -3556,19 +3373,16 @@
         <v>0</v>
       </c>
       <c r="I60">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J60">
-        <v>0</v>
-      </c>
-      <c r="K60">
-        <f t="shared" si="0"/>
-        <v>3.5209523809523806</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>5.0209523809523802</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B61">
         <v>243</v>
@@ -3592,19 +3406,16 @@
         <v>0</v>
       </c>
       <c r="I61">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="J61">
-        <v>0</v>
-      </c>
-      <c r="K61">
-        <f t="shared" si="0"/>
-        <v>3.47047619047619</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>5.5704761904761906</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B62">
         <v>243</v>
@@ -3628,19 +3439,16 @@
         <v>0</v>
       </c>
       <c r="I62">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="J62">
-        <v>0</v>
-      </c>
-      <c r="K62">
-        <f t="shared" si="0"/>
-        <v>1.7314285714285713</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>3.9314285714285715</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B63">
         <v>243</v>
@@ -3664,19 +3472,16 @@
         <v>0</v>
       </c>
       <c r="I63">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="J63">
-        <v>0</v>
-      </c>
-      <c r="K63">
-        <f t="shared" si="0"/>
-        <v>3.6714285714285713</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>6.0714285714285712</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B64">
         <v>243</v>
@@ -3700,19 +3505,16 @@
         <v>0</v>
       </c>
       <c r="I64">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="J64">
-        <v>0</v>
-      </c>
-      <c r="K64">
-        <f t="shared" si="0"/>
-        <v>3.5866666666666669</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>6.3866666666666667</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B65">
         <v>243</v>
@@ -3736,19 +3538,16 @@
         <v>0</v>
       </c>
       <c r="I65">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J65">
-        <v>0</v>
-      </c>
-      <c r="K65">
-        <f t="shared" si="0"/>
-        <v>3.6495238095238092</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>4.1495238095238092</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B66">
         <v>243</v>
@@ -3775,16 +3574,13 @@
         <v>0</v>
       </c>
       <c r="J66">
-        <v>0</v>
-      </c>
-      <c r="K66">
         <f t="shared" si="0"/>
         <v>2.9057142857142857</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B67">
         <v>243</v>
@@ -3808,19 +3604,16 @@
         <v>0</v>
       </c>
       <c r="I67">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J67">
-        <v>0</v>
-      </c>
-      <c r="K67">
-        <f t="shared" ref="K67:K106" si="1">MIN(10, 1+0.5*J67+0.2*I67+0.06*(C67/9+D67/7+E67/7+F67/7+G67/6))</f>
-        <v>3.6123809523809522</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" ref="J67:J72" si="1">MIN(10, 1+0.5*I67/5+0.2*H67+0.06*(C67/9+D67/7+E67/7+F67/7+G67/6))</f>
+        <v>4.6123809523809527</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B68">
         <v>243</v>
@@ -3844,19 +3637,16 @@
         <v>0</v>
       </c>
       <c r="I68">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="J68">
-        <v>0</v>
-      </c>
-      <c r="K68">
         <f t="shared" si="1"/>
-        <v>3.6257142857142854</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
+        <v>6.0257142857142849</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B69">
         <v>243</v>
@@ -3883,16 +3673,13 @@
         <v>0</v>
       </c>
       <c r="J69">
-        <v>0</v>
-      </c>
-      <c r="K69">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B70">
         <v>243</v>
@@ -3919,16 +3706,13 @@
         <v>0</v>
       </c>
       <c r="J70">
-        <v>0</v>
-      </c>
-      <c r="K70">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B71">
         <v>243</v>
@@ -3952,19 +3736,16 @@
         <v>0</v>
       </c>
       <c r="I71">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J71">
-        <v>0</v>
-      </c>
-      <c r="K71">
         <f t="shared" si="1"/>
-        <v>3.5933333333333333</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
+        <v>4.1933333333333334</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B72">
         <v>243</v>
@@ -3988,19 +3769,16 @@
         <v>0</v>
       </c>
       <c r="I72">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J72">
-        <v>0</v>
-      </c>
-      <c r="K72">
         <f t="shared" si="1"/>
-        <v>2.1314285714285717</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
+        <v>4.4314285714285715</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B73">
         <v>243</v>
@@ -4024,19 +3802,16 @@
         <v>0</v>
       </c>
       <c r="I73">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="J73">
-        <v>0</v>
-      </c>
-      <c r="K73">
-        <f t="shared" si="1"/>
-        <v>3.4942857142857142</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
+        <f>MIN(10, 1+0.5*I73/5+0.2*H73+0.06*(C73/9+D73/7+E73/7+F73/7+G73/6))</f>
+        <v>6.9942857142857147</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B74">
         <v>244</v>
@@ -4060,19 +3835,16 @@
         <v>0</v>
       </c>
       <c r="I74">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J74">
-        <v>0</v>
-      </c>
-      <c r="K74">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" ref="J74:J105" si="2">MIN(10, 1+0.5*I74/5+0.2*H74+0.06*(C74/9+D74/7+E74/7+F74/7+G74/6))</f>
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B75">
         <v>244</v>
@@ -4096,19 +3868,16 @@
         <v>0</v>
       </c>
       <c r="I75">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J75">
-        <v>0</v>
-      </c>
-      <c r="K75">
-        <f t="shared" si="1"/>
-        <v>2.1966666666666663</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>2.5966666666666667</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B76">
         <v>244</v>
@@ -4132,19 +3901,16 @@
         <v>0</v>
       </c>
       <c r="I76">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="J76">
-        <v>0</v>
-      </c>
-      <c r="K76">
-        <f t="shared" si="1"/>
-        <v>3.808095238095238</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>7.7080952380952379</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B77">
         <v>244</v>
@@ -4168,19 +3934,16 @@
         <v>0</v>
       </c>
       <c r="I77">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J77">
-        <v>0</v>
-      </c>
-      <c r="K77">
-        <f t="shared" si="1"/>
-        <v>2.1642857142857146</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>3.0642857142857141</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B78">
         <v>244</v>
@@ -4204,19 +3967,16 @@
         <v>0</v>
       </c>
       <c r="I78">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="J78">
-        <v>0</v>
-      </c>
-      <c r="K78">
-        <f t="shared" si="1"/>
-        <v>2.7671428571428573</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>4.6671428571428573</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B79">
         <v>244</v>
@@ -4240,19 +4000,16 @@
         <v>0</v>
       </c>
       <c r="I79">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="J79">
-        <v>0</v>
-      </c>
-      <c r="K79">
-        <f t="shared" si="1"/>
-        <v>3.652857142857143</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>5.8528571428571432</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B80">
         <v>244</v>
@@ -4276,19 +4033,16 @@
         <v>0</v>
       </c>
       <c r="I80">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J80">
-        <v>0</v>
-      </c>
-      <c r="K80">
-        <f t="shared" si="1"/>
-        <v>2.9428571428571426</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>4.5428571428571427</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B81">
         <v>244</v>
@@ -4312,19 +4066,16 @@
         <v>0</v>
       </c>
       <c r="I81">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="J81">
-        <v>0</v>
-      </c>
-      <c r="K81">
-        <f t="shared" si="1"/>
-        <v>3.583333333333333</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>5.7833333333333332</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B82">
         <v>244</v>
@@ -4348,19 +4099,16 @@
         <v>0</v>
       </c>
       <c r="I82">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J82">
-        <v>0</v>
-      </c>
-      <c r="K82">
-        <f t="shared" si="1"/>
-        <v>2.524285714285714</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>3.524285714285714</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B83">
         <v>244</v>
@@ -4387,16 +4135,13 @@
         <v>0</v>
       </c>
       <c r="J83">
-        <v>0</v>
-      </c>
-      <c r="K83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B84">
         <v>244</v>
@@ -4420,19 +4165,16 @@
         <v>0</v>
       </c>
       <c r="I84">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J84">
-        <v>0</v>
-      </c>
-      <c r="K84">
-        <f t="shared" si="1"/>
-        <v>3.4471428571428571</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>4.2471428571428573</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B85">
         <v>244</v>
@@ -4456,19 +4198,16 @@
         <v>0</v>
       </c>
       <c r="I85">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J85">
-        <v>0</v>
-      </c>
-      <c r="K85">
-        <f t="shared" si="1"/>
-        <v>3.4814285714285718</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>4.3814285714285717</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B86">
         <v>244</v>
@@ -4492,19 +4231,16 @@
         <v>0</v>
       </c>
       <c r="I86">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J86">
-        <v>0</v>
-      </c>
-      <c r="K86">
-        <f t="shared" si="1"/>
-        <v>2.5185714285714287</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>3.9185714285714282</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B87">
         <v>244</v>
@@ -4528,19 +4264,16 @@
         <v>0</v>
       </c>
       <c r="I87">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J87">
-        <v>0</v>
-      </c>
-      <c r="K87">
-        <f t="shared" si="1"/>
-        <v>1.6619047619047618</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>2.461904761904762</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B88">
         <v>244</v>
@@ -4564,19 +4297,16 @@
         <v>0</v>
       </c>
       <c r="I88">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J88">
-        <v>0</v>
-      </c>
-      <c r="K88">
-        <f t="shared" si="1"/>
-        <v>2.2619047619047619</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>3.0619047619047617</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B89">
         <v>244</v>
@@ -4600,19 +4330,16 @@
         <v>0</v>
       </c>
       <c r="I89">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="J89">
-        <v>0</v>
-      </c>
-      <c r="K89">
-        <f t="shared" si="1"/>
-        <v>3.7104761904761907</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>6.4104761904761904</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B90">
         <v>244</v>
@@ -4636,19 +4363,16 @@
         <v>0</v>
       </c>
       <c r="I90">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J90">
-        <v>0</v>
-      </c>
-      <c r="K90">
-        <f t="shared" si="1"/>
-        <v>3.2766666666666664</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>4.7766666666666664</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B91">
         <v>244</v>
@@ -4672,19 +4396,16 @@
         <v>0</v>
       </c>
       <c r="I91">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J91">
-        <v>0</v>
-      </c>
-      <c r="K91">
-        <f t="shared" si="1"/>
-        <v>2.7790476190476188</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>4.3790476190476193</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B92">
         <v>244</v>
@@ -4708,19 +4429,16 @@
         <v>0</v>
       </c>
       <c r="I92">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="J92">
-        <v>0</v>
-      </c>
-      <c r="K92">
-        <f t="shared" si="1"/>
-        <v>3.7190476190476187</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>7.019047619047619</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B93">
         <v>244</v>
@@ -4744,19 +4462,16 @@
         <v>0</v>
       </c>
       <c r="I93">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="J93">
-        <v>0</v>
-      </c>
-      <c r="K93">
-        <f t="shared" si="1"/>
-        <v>3.7352380952380946</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>7.4352380952380948</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B94">
         <v>244</v>
@@ -4780,19 +4495,16 @@
         <v>0</v>
       </c>
       <c r="I94">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J94">
-        <v>0</v>
-      </c>
-      <c r="K94">
-        <f t="shared" si="1"/>
-        <v>2.9538095238095234</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>4.4538095238095234</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B95">
         <v>244</v>
@@ -4816,19 +4528,16 @@
         <v>0</v>
       </c>
       <c r="I95">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J95">
-        <v>0</v>
-      </c>
-      <c r="K95">
-        <f t="shared" si="1"/>
-        <v>3.2833333333333332</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>5.583333333333333</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B96">
         <v>244</v>
@@ -4852,19 +4561,16 @@
         <v>0</v>
       </c>
       <c r="I96">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="J96">
-        <v>0</v>
-      </c>
-      <c r="K96">
-        <f t="shared" si="1"/>
-        <v>3.6547619047619051</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>5.7547619047619047</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B97">
         <v>244</v>
@@ -4888,19 +4594,16 @@
         <v>0</v>
       </c>
       <c r="I97">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J97">
-        <v>0</v>
-      </c>
-      <c r="K97">
-        <f t="shared" si="1"/>
-        <v>3.494761904761905</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>4.2947619047619048</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B98">
         <v>244</v>
@@ -4924,19 +4627,16 @@
         <v>0</v>
       </c>
       <c r="I98">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J98">
-        <v>0</v>
-      </c>
-      <c r="K98">
-        <f t="shared" si="1"/>
-        <v>3.67</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>4.57</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B99">
         <v>244</v>
@@ -4960,19 +4660,16 @@
         <v>0</v>
       </c>
       <c r="I99">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J99">
-        <v>0</v>
-      </c>
-      <c r="K99">
-        <f t="shared" si="1"/>
-        <v>3.0295238095238095</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>4.4295238095238094</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B100">
         <v>244</v>
@@ -4996,19 +4693,16 @@
         <v>0</v>
       </c>
       <c r="I100">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="J100">
-        <v>0</v>
-      </c>
-      <c r="K100">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B101">
         <v>244</v>
@@ -5032,19 +4726,16 @@
         <v>0</v>
       </c>
       <c r="I101">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="J101">
-        <v>0</v>
-      </c>
-      <c r="K101">
-        <f t="shared" si="1"/>
-        <v>3.671904761904762</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>6.4719047619047618</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B102">
         <v>244</v>
@@ -5068,19 +4759,16 @@
         <v>0</v>
       </c>
       <c r="I102">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="J102">
-        <v>0</v>
-      </c>
-      <c r="K102">
-        <f t="shared" si="1"/>
-        <v>3.6357142857142857</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>7.4357142857142851</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B103">
         <v>244</v>
@@ -5104,19 +4792,16 @@
         <v>0</v>
       </c>
       <c r="I103">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J103">
-        <v>0</v>
-      </c>
-      <c r="K103">
-        <f t="shared" si="1"/>
-        <v>2.7585714285714285</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>3.7585714285714285</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B104">
         <v>244</v>
@@ -5140,19 +4825,16 @@
         <v>0</v>
       </c>
       <c r="I104">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="J104">
-        <v>0</v>
-      </c>
-      <c r="K104">
-        <f t="shared" si="1"/>
-        <v>3.2899999999999996</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>5.89</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B105">
         <v>244</v>
@@ -5179,16 +4861,13 @@
         <v>0</v>
       </c>
       <c r="J105">
-        <v>0</v>
-      </c>
-      <c r="K105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.85</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B106">
         <v>241</v>
@@ -5212,18 +4891,15 @@
         <v>0</v>
       </c>
       <c r="I106">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J106">
-        <v>0</v>
-      </c>
-      <c r="K106">
-        <f t="shared" si="1"/>
-        <v>2.3714285714285714</v>
+        <f>MIN(10, 1+0.5*I106/5+0.2*H106+0.06*(C106/9+D106/7+E106/7+F106/7+G106/6))</f>
+        <v>3.1714285714285717</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K106" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:J106" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Results PS - preliminary
</commit_message>
<xml_diff>
--- a/Teaching/2017-2018/PS web page/results/Tabel_Prob_Stat.xlsx
+++ b/Teaching/2017-2018/PS web page/results/Tabel_Prob_Stat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amari\OneDrive\GitHub\AlexAmarioarei.github.io\Teaching\2017-2018\PS web page\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="8FF3444C7F665870D3AD9D990F8B37298E07E54C" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{B201E90F-CCF8-423C-9691-9374B0CB9082}"/>
+  <xr:revisionPtr revIDLastSave="224" documentId="8FF3444C7F665870D3AD9D990F8B37298E07E54C" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{B90587DD-658A-42D0-B8D7-DA1DA6AE7717}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13815" windowHeight="10605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -507,7 +507,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -687,6 +687,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -848,8 +854,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -895,7 +902,15 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1393,10 +1408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J106"/>
+  <dimension ref="A1:L106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I76" sqref="I76"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1404,7 +1419,7 @@
     <col min="1" max="1" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1436,7 +1451,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1459,17 +1474,21 @@
         <v>54</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="I2">
         <v>31</v>
       </c>
       <c r="J2">
-        <f>MIN(10, 1+0.5*I2/5+0.2*H2+0.06*(C2/9+D2/7+E2/7+F2/7+G2/6))</f>
-        <v>6.7323809523809519</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+        <f>MAX(4, ROUND(MIN(10, 1+0.5*I2/5+0.2*H2/10+0.06*(C2/9+D2/7+E2/7+F2/7+G2/6)),0))</f>
+        <v>8</v>
+      </c>
+      <c r="L2">
+        <f>MIN(10, 1+0.5*I2/5+0.2*H2/10+0.06*(C2/9+D2/7+E2/7+F2/7+G2/6))</f>
+        <v>8.432380952380953</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1492,17 +1511,21 @@
         <v>47</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="I3">
         <v>25</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J66" si="0">MIN(10, 1+0.5*I3/5+0.2*H3+0.06*(C3/9+D3/7+E3/7+F3/7+G3/6))</f>
-        <v>5.7976190476190474</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+        <f t="shared" ref="J3:J66" si="0">MAX(4, ROUND(MIN(10, 1+0.5*I3/5+0.2*H3/10+0.06*(C3/9+D3/7+E3/7+F3/7+G3/6)),0))</f>
+        <v>7</v>
+      </c>
+      <c r="L3">
+        <f>MIN(10, 1+0.5*I3/5+0.2*H3/10+0.06*(C3/9+D3/7+E3/7+F3/7+G3/6))</f>
+        <v>7.1376190476190473</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1525,17 +1548,21 @@
         <v>55</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I4">
         <v>17</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>5.1071428571428577</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L67" si="1">MIN(10, 1+0.5*I4/5+0.2*H4/10+0.06*(C4/9+D4/7+E4/7+F4/7+G4/6))</f>
+        <v>6.1071428571428577</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1558,17 +1585,21 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="I5">
         <v>7</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>2.1466666666666665</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>3.3666666666666667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1591,17 +1622,21 @@
         <v>51</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="I6">
         <v>12</v>
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>3.9604761904761907</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>5.1204761904761913</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1624,17 +1659,21 @@
         <v>46</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="I7">
         <v>20</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>4.9828571428571431</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>6.1428571428571432</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1657,17 +1696,21 @@
         <v>53</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="I8">
         <v>21</v>
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>4.55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>5.41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1697,10 +1740,14 @@
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
         <v>1.7819047619047619</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1723,17 +1770,21 @@
         <v>56</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10">
         <f t="shared" si="0"/>
-        <v>3.0552380952380953</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" si="1"/>
+        <v>4.2752380952380955</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1756,17 +1807,21 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1789,17 +1844,21 @@
         <v>40</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="I12">
         <v>14</v>
       </c>
       <c r="J12">
         <f t="shared" si="0"/>
-        <v>4.2085714285714282</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>4.8885714285714288</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1822,17 +1881,21 @@
         <v>55</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="I13">
         <v>21</v>
       </c>
       <c r="J13">
         <f t="shared" si="0"/>
-        <v>5.6595238095238098</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>7.3595238095238091</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1854,15 +1917,22 @@
       <c r="G14">
         <v>55</v>
       </c>
+      <c r="H14">
+        <v>82</v>
+      </c>
       <c r="I14">
         <v>25</v>
       </c>
       <c r="J14">
         <f t="shared" si="0"/>
-        <v>6.121428571428571</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>7.7614285714285716</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1885,17 +1955,21 @@
         <v>48</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>3.1409523809523812</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>4.7809523809523817</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1918,17 +1992,21 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="I16">
         <v>19</v>
       </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>3.4085714285714284</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="1"/>
+        <v>4.6885714285714286</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1951,17 +2029,21 @@
         <v>41</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="I17">
         <v>13</v>
       </c>
       <c r="J17">
         <f t="shared" si="0"/>
-        <v>3.4099999999999997</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" si="1"/>
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1984,17 +2066,21 @@
         <v>53</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I18">
         <v>18</v>
       </c>
       <c r="J18">
         <f t="shared" si="0"/>
-        <v>5.4014285714285712</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="1"/>
+        <v>6.4014285714285712</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -2017,17 +2103,21 @@
         <v>47</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="I19">
         <v>20</v>
       </c>
       <c r="J19">
         <f t="shared" si="0"/>
-        <v>4.7519047619047621</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="1"/>
+        <v>5.4719047619047618</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -2057,10 +2147,14 @@
       </c>
       <c r="J20">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -2083,17 +2177,21 @@
         <v>54</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="I21">
         <v>21</v>
       </c>
       <c r="J21">
         <f t="shared" si="0"/>
-        <v>5.7866666666666671</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="1"/>
+        <v>7.4866666666666664</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -2123,10 +2221,14 @@
       </c>
       <c r="J22">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -2149,17 +2251,21 @@
         <v>48</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="I23">
         <v>19</v>
       </c>
       <c r="J23">
         <f t="shared" si="0"/>
-        <v>5.3647619047619042</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="1"/>
+        <v>6.0847619047619048</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -2182,17 +2288,21 @@
         <v>0</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="I24">
         <v>10</v>
       </c>
       <c r="J24">
         <f t="shared" si="0"/>
-        <v>3.097142857142857</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="1"/>
+        <v>4.4371428571428568</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -2222,10 +2332,14 @@
       </c>
       <c r="J25">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="1"/>
         <v>2.9685714285714284</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -2248,17 +2362,21 @@
         <v>44</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I26">
         <v>0</v>
       </c>
       <c r="J26">
         <f t="shared" si="0"/>
-        <v>2.5419047619047621</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="1"/>
+        <v>3.1419047619047618</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -2281,17 +2399,21 @@
         <v>52</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="I27">
         <v>20</v>
       </c>
       <c r="J27">
         <f t="shared" si="0"/>
-        <v>4.8199999999999994</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="1"/>
+        <v>5.8999999999999995</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -2314,17 +2436,21 @@
         <v>45</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="I28">
         <v>9</v>
       </c>
       <c r="J28">
         <f t="shared" si="0"/>
-        <v>4.3699999999999992</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="1"/>
+        <v>5.4499999999999993</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -2347,17 +2473,21 @@
         <v>0</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="I29">
         <v>14</v>
       </c>
       <c r="J29">
         <f t="shared" si="0"/>
-        <v>4.4847619047619052</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="1"/>
+        <v>5.5647619047619052</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -2387,10 +2517,14 @@
       </c>
       <c r="J30">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="1"/>
         <v>2.2104761904761903</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -2413,17 +2547,21 @@
         <v>52</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="I31">
         <v>19</v>
       </c>
       <c r="J31">
         <f t="shared" si="0"/>
-        <v>4.92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="1"/>
+        <v>6.0399999999999991</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -2453,10 +2591,14 @@
       </c>
       <c r="J32">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="1"/>
         <v>1.5161904761904763</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -2479,17 +2621,21 @@
         <v>52</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="I33">
         <v>22</v>
       </c>
       <c r="J33">
         <f t="shared" si="0"/>
-        <v>5.0247619047619043</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="1"/>
+        <v>6.1047619047619044</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -2512,17 +2658,21 @@
         <v>51</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="I34">
         <v>21</v>
       </c>
       <c r="J34">
         <f t="shared" si="0"/>
-        <v>5.2671428571428578</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="1"/>
+        <v>5.6871428571428577</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -2545,17 +2695,21 @@
         <v>52</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="I35">
         <v>17</v>
       </c>
       <c r="J35">
         <f t="shared" si="0"/>
-        <v>4.9857142857142858</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="1"/>
+        <v>5.4057142857142857</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -2585,10 +2739,14 @@
       </c>
       <c r="J36">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="1"/>
         <v>3.1714285714285713</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -2618,10 +2776,14 @@
       </c>
       <c r="J37">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -2644,17 +2806,21 @@
         <v>52</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="I38">
         <v>10</v>
       </c>
       <c r="J38">
         <f t="shared" si="0"/>
-        <v>4.0457142857142863</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="1"/>
+        <v>5.1657142857142855</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -2684,10 +2850,14 @@
       </c>
       <c r="J39">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="1"/>
         <v>1.9157142857142857</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -2710,17 +2880,21 @@
         <v>53</v>
       </c>
       <c r="H40">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="I40">
         <v>20</v>
       </c>
       <c r="J40">
         <f t="shared" si="0"/>
-        <v>5.5823809523809516</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="1"/>
+        <v>6.9223809523809514</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -2750,10 +2924,14 @@
       </c>
       <c r="J41">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="1"/>
         <v>2.1890476190476189</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -2776,17 +2954,21 @@
         <v>27</v>
       </c>
       <c r="H42">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I42">
         <v>16</v>
       </c>
       <c r="J42">
         <f t="shared" si="0"/>
-        <v>4.2166666666666668</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="1"/>
+        <v>4.4366666666666665</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -2816,10 +2998,14 @@
       </c>
       <c r="J43">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -2849,10 +3035,14 @@
       </c>
       <c r="J44">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="1"/>
         <v>2.0123809523809522</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -2875,17 +3065,21 @@
         <v>0</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="I45">
         <v>18</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
-        <v>4.6628571428571428</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="1"/>
+        <v>5.7428571428571429</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>54</v>
       </c>
@@ -2908,17 +3102,21 @@
         <v>53</v>
       </c>
       <c r="H46">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="I46">
         <v>22</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>5.3138095238095246</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="1"/>
+        <v>6.3938095238095247</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -2941,17 +3139,21 @@
         <v>53</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="I47">
         <v>30</v>
       </c>
       <c r="J47">
         <f t="shared" si="0"/>
-        <v>6.6109523809523809</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="1"/>
+        <v>7.9509523809523808</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -2981,10 +3183,14 @@
       </c>
       <c r="J48">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="1"/>
         <v>2.0152380952380953</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -3007,17 +3213,21 @@
         <v>0</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="I49">
         <v>14</v>
       </c>
       <c r="J49">
         <f t="shared" si="0"/>
-        <v>3.4285714285714284</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="1"/>
+        <v>4.5085714285714289</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -3040,17 +3250,21 @@
         <v>51</v>
       </c>
       <c r="H50">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="I50">
         <v>28</v>
       </c>
       <c r="J50">
         <f t="shared" si="0"/>
-        <v>6.2042857142857137</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="1"/>
+        <v>7.0842857142857136</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -3080,10 +3294,14 @@
       </c>
       <c r="J51">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -3106,17 +3324,21 @@
         <v>52</v>
       </c>
       <c r="H52">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="I52">
         <v>21</v>
       </c>
       <c r="J52">
         <f t="shared" si="0"/>
-        <v>5.2295238095238092</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="1"/>
+        <v>6.9095238095238098</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>61</v>
       </c>
@@ -3139,17 +3361,21 @@
         <v>52</v>
       </c>
       <c r="H53">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="I53">
         <v>27</v>
       </c>
       <c r="J53">
         <f t="shared" si="0"/>
-        <v>6.3009523809523813</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="1"/>
+        <v>7.7009523809523799</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>62</v>
       </c>
@@ -3179,10 +3405,14 @@
       </c>
       <c r="J54">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="1"/>
         <v>1.48</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -3205,17 +3435,21 @@
         <v>0</v>
       </c>
       <c r="H55">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="I55">
         <v>26</v>
       </c>
       <c r="J55">
         <f t="shared" si="0"/>
-        <v>4.9419047619047625</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="1"/>
+        <v>5.961904761904762</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>64</v>
       </c>
@@ -3238,17 +3472,21 @@
         <v>52</v>
       </c>
       <c r="H56">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="I56">
         <v>28</v>
       </c>
       <c r="J56">
         <f t="shared" si="0"/>
-        <v>6.1571428571428566</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="1"/>
+        <v>7.4171428571428581</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>65</v>
       </c>
@@ -3271,17 +3509,21 @@
         <v>0</v>
       </c>
       <c r="H57">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="I57">
         <v>20</v>
       </c>
       <c r="J57">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="1"/>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>66</v>
       </c>
@@ -3304,17 +3546,21 @@
         <v>0</v>
       </c>
       <c r="H58">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="I58">
         <v>4</v>
       </c>
       <c r="J58">
         <f t="shared" si="0"/>
-        <v>1.9495238095238094</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="1"/>
+        <v>2.5695238095238095</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>67</v>
       </c>
@@ -3337,17 +3583,21 @@
         <v>0</v>
       </c>
       <c r="H59">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="I59">
         <v>20</v>
       </c>
       <c r="J59">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="1"/>
+        <v>4.08</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -3370,17 +3620,21 @@
         <v>52</v>
       </c>
       <c r="H60">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="I60">
         <v>15</v>
       </c>
       <c r="J60">
         <f t="shared" si="0"/>
-        <v>5.0209523809523802</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="1"/>
+        <v>6.7009523809523799</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>69</v>
       </c>
@@ -3403,17 +3657,21 @@
         <v>52</v>
       </c>
       <c r="H61">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="I61">
         <v>21</v>
       </c>
       <c r="J61">
         <f t="shared" si="0"/>
-        <v>5.5704761904761906</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="1"/>
+        <v>6.5904761904761902</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -3443,10 +3701,14 @@
       </c>
       <c r="J62">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="1"/>
         <v>3.9314285714285715</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>71</v>
       </c>
@@ -3469,17 +3731,21 @@
         <v>52</v>
       </c>
       <c r="H63">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="I63">
         <v>24</v>
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>6.0714285714285712</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="1"/>
+        <v>6.7914285714285718</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>72</v>
       </c>
@@ -3502,17 +3768,21 @@
         <v>52</v>
       </c>
       <c r="H64">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="I64">
         <v>28</v>
       </c>
       <c r="J64">
         <f t="shared" si="0"/>
-        <v>6.3866666666666667</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="1"/>
+        <v>8.1066666666666656</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>73</v>
       </c>
@@ -3535,17 +3805,21 @@
         <v>52</v>
       </c>
       <c r="H65">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="I65">
         <v>5</v>
       </c>
       <c r="J65">
         <f t="shared" si="0"/>
-        <v>4.1495238095238092</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="1"/>
+        <v>5.2495238095238097</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>74</v>
       </c>
@@ -3568,17 +3842,21 @@
         <v>52</v>
       </c>
       <c r="H66">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="I66">
         <v>0</v>
       </c>
       <c r="J66">
         <f t="shared" si="0"/>
-        <v>2.9057142857142857</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="L66">
+        <f t="shared" si="1"/>
+        <v>3.6257142857142854</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>75</v>
       </c>
@@ -3601,17 +3879,21 @@
         <v>52</v>
       </c>
       <c r="H67">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="I67">
         <v>10</v>
       </c>
       <c r="J67">
-        <f t="shared" ref="J67:J72" si="1">MIN(10, 1+0.5*I67/5+0.2*H67+0.06*(C67/9+D67/7+E67/7+F67/7+G67/6))</f>
-        <v>4.6123809523809527</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
+        <f t="shared" ref="J67:J106" si="2">MAX(4, ROUND(MIN(10, 1+0.5*I67/5+0.2*H67/10+0.06*(C67/9+D67/7+E67/7+F67/7+G67/6)),0))</f>
+        <v>5</v>
+      </c>
+      <c r="L67">
+        <f t="shared" si="1"/>
+        <v>5.4923809523809517</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>76</v>
       </c>
@@ -3634,17 +3916,21 @@
         <v>52</v>
       </c>
       <c r="H68">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="I68">
         <v>24</v>
       </c>
       <c r="J68">
-        <f t="shared" si="1"/>
-        <v>6.0257142857142849</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="L68">
+        <f t="shared" ref="L68:L106" si="3">MIN(10, 1+0.5*I68/5+0.2*H68/10+0.06*(C68/9+D68/7+E68/7+F68/7+G68/6))</f>
+        <v>7.7457142857142856</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>77</v>
       </c>
@@ -3673,11 +3959,15 @@
         <v>0</v>
       </c>
       <c r="J69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>78</v>
       </c>
@@ -3706,11 +3996,15 @@
         <v>0</v>
       </c>
       <c r="J70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>79</v>
       </c>
@@ -3733,17 +4027,21 @@
         <v>52</v>
       </c>
       <c r="H71">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="I71">
         <v>6</v>
       </c>
       <c r="J71">
-        <f t="shared" si="1"/>
-        <v>4.1933333333333334</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="L71">
+        <f t="shared" si="3"/>
+        <v>5.293333333333333</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>80</v>
       </c>
@@ -3766,17 +4064,21 @@
         <v>0</v>
       </c>
       <c r="H72">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="I72">
         <v>23</v>
       </c>
       <c r="J72">
-        <f t="shared" si="1"/>
-        <v>4.4314285714285715</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="3"/>
+        <v>5.6914285714285722</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>81</v>
       </c>
@@ -3799,17 +4101,21 @@
         <v>52</v>
       </c>
       <c r="H73">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="I73">
         <v>35</v>
       </c>
       <c r="J73">
-        <f>MIN(10, 1+0.5*I73/5+0.2*H73+0.06*(C73/9+D73/7+E73/7+F73/7+G73/6))</f>
-        <v>6.9942857142857147</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="3"/>
+        <v>8.5942857142857143</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>82</v>
       </c>
@@ -3832,17 +4138,21 @@
         <v>0</v>
       </c>
       <c r="H74">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="I74">
         <v>9</v>
       </c>
       <c r="J74">
-        <f t="shared" ref="J74:J105" si="2">MIN(10, 1+0.5*I74/5+0.2*H74+0.06*(C74/9+D74/7+E74/7+F74/7+G74/6))</f>
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="L74">
+        <f t="shared" si="3"/>
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>83</v>
       </c>
@@ -3865,17 +4175,21 @@
         <v>53</v>
       </c>
       <c r="H75">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I75">
         <v>4</v>
       </c>
       <c r="J75">
         <f t="shared" si="2"/>
-        <v>2.5966666666666667</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="L75">
+        <f t="shared" si="3"/>
+        <v>2.8566666666666665</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>84</v>
       </c>
@@ -3898,17 +4212,21 @@
         <v>57</v>
       </c>
       <c r="H76">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="I76">
         <v>39</v>
       </c>
       <c r="J76">
         <f t="shared" si="2"/>
-        <v>7.7080952380952379</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
+        <v>10</v>
+      </c>
+      <c r="L76">
+        <f t="shared" si="3"/>
+        <v>9.6080952380952382</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>85</v>
       </c>
@@ -3931,17 +4249,21 @@
         <v>47</v>
       </c>
       <c r="H77">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="I77">
         <v>9</v>
       </c>
       <c r="J77">
         <f t="shared" si="2"/>
-        <v>3.0642857142857141</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="L77">
+        <f t="shared" si="3"/>
+        <v>4.5442857142857145</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>86</v>
       </c>
@@ -3964,17 +4286,21 @@
         <v>53</v>
       </c>
       <c r="H78">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="I78">
         <v>19</v>
       </c>
       <c r="J78">
         <f t="shared" si="2"/>
-        <v>4.6671428571428573</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="L78">
+        <f t="shared" si="3"/>
+        <v>6.2471428571428582</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>87</v>
       </c>
@@ -3997,17 +4323,21 @@
         <v>53</v>
       </c>
       <c r="H79">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="I79">
         <v>22</v>
       </c>
       <c r="J79">
         <f t="shared" si="2"/>
-        <v>5.8528571428571432</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="L79">
+        <f t="shared" si="3"/>
+        <v>7.4328571428571433</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>88</v>
       </c>
@@ -4030,17 +4360,21 @@
         <v>52</v>
       </c>
       <c r="H80">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="I80">
         <v>16</v>
       </c>
       <c r="J80">
         <f t="shared" si="2"/>
-        <v>4.5428571428571427</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="L80">
+        <f t="shared" si="3"/>
+        <v>5.9628571428571426</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>89</v>
       </c>
@@ -4063,17 +4397,21 @@
         <v>49</v>
       </c>
       <c r="H81">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="I81">
         <v>22</v>
       </c>
       <c r="J81">
         <f t="shared" si="2"/>
-        <v>5.7833333333333332</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="L81">
+        <f t="shared" si="3"/>
+        <v>7.3833333333333337</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>90</v>
       </c>
@@ -4096,17 +4434,21 @@
         <v>53</v>
       </c>
       <c r="H82">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="I82">
         <v>10</v>
       </c>
       <c r="J82">
         <f t="shared" si="2"/>
-        <v>3.524285714285714</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="L82">
+        <f t="shared" si="3"/>
+        <v>4.6442857142857141</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>91</v>
       </c>
@@ -4136,10 +4478,14 @@
       </c>
       <c r="J83">
         <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="L83">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>92</v>
       </c>
@@ -4162,17 +4508,21 @@
         <v>53</v>
       </c>
       <c r="H84">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="I84">
         <v>8</v>
       </c>
       <c r="J84">
         <f t="shared" si="2"/>
-        <v>4.2471428571428573</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="L84">
+        <f t="shared" si="3"/>
+        <v>5.7271428571428569</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>93</v>
       </c>
@@ -4195,17 +4545,21 @@
         <v>53</v>
       </c>
       <c r="H85">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="I85">
         <v>9</v>
       </c>
       <c r="J85">
         <f t="shared" si="2"/>
-        <v>4.3814285714285717</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="L85">
+        <f t="shared" si="3"/>
+        <v>5.8814285714285717</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>94</v>
       </c>
@@ -4228,17 +4582,21 @@
         <v>53</v>
       </c>
       <c r="H86">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="I86">
         <v>14</v>
       </c>
       <c r="J86">
         <f t="shared" si="2"/>
-        <v>3.9185714285714282</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="L86">
+        <f t="shared" si="3"/>
+        <v>5.338571428571429</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>95</v>
       </c>
@@ -4261,17 +4619,21 @@
         <v>0</v>
       </c>
       <c r="H87">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="I87">
         <v>8</v>
       </c>
       <c r="J87">
         <f t="shared" si="2"/>
-        <v>2.461904761904762</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="L87">
+        <f t="shared" si="3"/>
+        <v>3.5819047619047617</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>96</v>
       </c>
@@ -4294,17 +4656,21 @@
         <v>0</v>
       </c>
       <c r="H88">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="I88">
         <v>8</v>
       </c>
       <c r="J88">
         <f t="shared" si="2"/>
-        <v>3.0619047619047617</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="L88">
+        <f t="shared" si="3"/>
+        <v>4.5019047619047621</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>97</v>
       </c>
@@ -4327,17 +4693,21 @@
         <v>54</v>
       </c>
       <c r="H89">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="I89">
         <v>27</v>
       </c>
       <c r="J89">
         <f t="shared" si="2"/>
-        <v>6.4104761904761904</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+      <c r="L89">
+        <f t="shared" si="3"/>
+        <v>8.1104761904761915</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>98</v>
       </c>
@@ -4360,17 +4730,21 @@
         <v>53</v>
       </c>
       <c r="H90">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="I90">
         <v>15</v>
       </c>
       <c r="J90">
         <f t="shared" si="2"/>
-        <v>4.7766666666666664</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="L90">
+        <f t="shared" si="3"/>
+        <v>6.2766666666666664</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>99</v>
       </c>
@@ -4393,17 +4767,21 @@
         <v>0</v>
       </c>
       <c r="H91">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="I91">
         <v>16</v>
       </c>
       <c r="J91">
         <f t="shared" si="2"/>
-        <v>4.3790476190476193</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="L91">
+        <f t="shared" si="3"/>
+        <v>5.8190476190476188</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>100</v>
       </c>
@@ -4426,17 +4804,21 @@
         <v>52</v>
       </c>
       <c r="H92">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="I92">
         <v>33</v>
       </c>
       <c r="J92">
         <f t="shared" si="2"/>
-        <v>7.019047619047619</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="L92">
+        <f t="shared" si="3"/>
+        <v>8.5390476190476186</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>101</v>
       </c>
@@ -4459,17 +4841,21 @@
         <v>54</v>
       </c>
       <c r="H93">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="I93">
         <v>37</v>
       </c>
       <c r="J93">
         <f t="shared" si="2"/>
-        <v>7.4352380952380948</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="L93">
+        <f t="shared" si="3"/>
+        <v>9.3352380952380933</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>102</v>
       </c>
@@ -4492,17 +4878,21 @@
         <v>53</v>
       </c>
       <c r="H94">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="I94">
         <v>15</v>
       </c>
       <c r="J94">
         <f t="shared" si="2"/>
-        <v>4.4538095238095234</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="L94">
+        <f t="shared" si="3"/>
+        <v>5.6538095238095236</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>103</v>
       </c>
@@ -4525,17 +4915,21 @@
         <v>53</v>
       </c>
       <c r="H95">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="I95">
         <v>23</v>
       </c>
       <c r="J95">
         <f t="shared" si="2"/>
-        <v>5.583333333333333</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="L95">
+        <f t="shared" si="3"/>
+        <v>7.1833333333333336</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>77</v>
       </c>
@@ -4558,17 +4952,21 @@
         <v>53</v>
       </c>
       <c r="H96">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="I96">
         <v>21</v>
       </c>
       <c r="J96">
         <f t="shared" si="2"/>
-        <v>5.7547619047619047</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="L96">
+        <f t="shared" si="3"/>
+        <v>7.3347619047619048</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>104</v>
       </c>
@@ -4591,17 +4989,21 @@
         <v>53</v>
       </c>
       <c r="H97">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="I97">
         <v>8</v>
       </c>
       <c r="J97">
         <f t="shared" si="2"/>
-        <v>4.2947619047619048</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="L97">
+        <f t="shared" si="3"/>
+        <v>5.4747619047619054</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>105</v>
       </c>
@@ -4624,17 +5026,21 @@
         <v>53</v>
       </c>
       <c r="H98">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="I98">
         <v>9</v>
       </c>
       <c r="J98">
         <f t="shared" si="2"/>
-        <v>4.57</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="L98">
+        <f t="shared" si="3"/>
+        <v>5.81</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>106</v>
       </c>
@@ -4657,17 +5063,21 @@
         <v>52</v>
       </c>
       <c r="H99">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="I99">
         <v>14</v>
       </c>
       <c r="J99">
         <f t="shared" si="2"/>
-        <v>4.4295238095238094</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="L99">
+        <f t="shared" si="3"/>
+        <v>5.5495238095238095</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>107</v>
       </c>
@@ -4690,17 +5100,21 @@
         <v>0</v>
       </c>
       <c r="H100">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="I100">
         <v>19</v>
       </c>
       <c r="J100">
         <f t="shared" si="2"/>
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="L100">
+        <f t="shared" si="3"/>
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>108</v>
       </c>
@@ -4723,17 +5137,21 @@
         <v>53</v>
       </c>
       <c r="H101">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="I101">
         <v>28</v>
       </c>
       <c r="J101">
         <f t="shared" si="2"/>
-        <v>6.4719047619047618</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+      <c r="L101">
+        <f t="shared" si="3"/>
+        <v>7.9919047619047623</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>109</v>
       </c>
@@ -4756,17 +5174,21 @@
         <v>53</v>
       </c>
       <c r="H102">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="I102">
         <v>38</v>
       </c>
       <c r="J102">
         <f t="shared" si="2"/>
-        <v>7.4357142857142851</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="L102">
+        <f t="shared" si="3"/>
+        <v>9.0357142857142865</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>110</v>
       </c>
@@ -4789,17 +5211,21 @@
         <v>53</v>
       </c>
       <c r="H103">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="I103">
         <v>10</v>
       </c>
       <c r="J103">
         <f t="shared" si="2"/>
-        <v>3.7585714285714285</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+      <c r="L103">
+        <f t="shared" si="3"/>
+        <v>4.9385714285714286</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>111</v>
       </c>
@@ -4822,17 +5248,21 @@
         <v>51</v>
       </c>
       <c r="H104">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="I104">
         <v>26</v>
       </c>
       <c r="J104">
         <f t="shared" si="2"/>
-        <v>5.89</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+      <c r="L104">
+        <f t="shared" si="3"/>
+        <v>7.4699999999999989</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>112</v>
       </c>
@@ -4855,17 +5285,21 @@
         <v>37</v>
       </c>
       <c r="H105">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="I105">
         <v>0</v>
       </c>
       <c r="J105">
         <f t="shared" si="2"/>
-        <v>1.85</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="L105">
+        <f t="shared" si="3"/>
+        <v>3.0900000000000003</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>113</v>
       </c>
@@ -4894,13 +5328,24 @@
         <v>8</v>
       </c>
       <c r="J106">
-        <f>MIN(10, 1+0.5*I106/5+0.2*H106+0.06*(C106/9+D106/7+E106/7+F106/7+G106/6))</f>
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="L106">
+        <f t="shared" si="3"/>
         <v>3.1714285714285717</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J106" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+      <formula>4.05</formula>
+      <formula>4.49</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>